<commit_message>
Primera edicion de datos
</commit_message>
<xml_diff>
--- a/md101/Productos.xlsx
+++ b/md101/Productos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaveza\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DJCA\utec\dev\data\md101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53077018-33BD-49A0-9F7F-2B3F9DC9BFC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A232FC-9F16-466F-9723-02FB487556A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="96" windowWidth="23892" windowHeight="14532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,11 +612,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" customWidth="1"/>
   </cols>

</xml_diff>